<commit_message>
Translate readme, Process XLS files and file names
</commit_message>
<xml_diff>
--- a/6.Process/BOM/mpu6050.xlsx
+++ b/6.Process/BOM/mpu6050.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Cubli_Mini\6.Process\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\data\Projects\others\Cubli\CubliMini\6.Process\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A049F4D3-21C3-45A2-AF33-828D8E8DEBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A98C70C-B4DE-405D-AC24-341D139E8491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mpu6050" sheetId="1" r:id="rId1"/>
@@ -38,17 +38,6 @@
   </si>
   <si>
     <t>Quantity</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>途径</t>
-    </r>
   </si>
   <si>
     <r>
@@ -91,17 +80,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>贴片电容</t>
-    </r>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -111,17 +89,6 @@
     <t>0402 100nF (104) 10% 16V</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>立创商城</t>
-    </r>
-  </si>
-  <si>
     <t>10nF (103) 10% 50V</t>
   </si>
   <si>
@@ -161,17 +128,6 @@
     <t>0Ω (0R0) ±1%</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>贴片电阻</t>
-    </r>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
@@ -206,17 +162,6 @@
   </si>
   <si>
     <t>QFN-24_L4.0-W4.0-P0.50-BL-EP2.6</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>淘宝</t>
-    </r>
   </si>
   <si>
     <t>https://item.szlcsc.com/61185.html</t>
@@ -253,17 +198,32 @@
   <si>
     <t>https://item.szlcsc.com/306650.html</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SMD capacitor</t>
+  </si>
+  <si>
+    <t>SMD resistor</t>
+  </si>
+  <si>
+    <t>Taobao</t>
+  </si>
+  <si>
+    <t>LCSC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -277,7 +237,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -289,7 +249,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -297,7 +257,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -402,8 +362,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -678,18 +638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="15.625" customWidth="1"/>
-    <col min="8" max="8" width="95.375" customWidth="1"/>
+    <col min="1" max="6" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="95.42578125" customWidth="1"/>
     <col min="9" max="9" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -709,245 +667,245 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E5" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="F8" s="3">
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>